<commit_message>
Slight changes made to codeBook and DataCollectionTemplate
</commit_message>
<xml_diff>
--- a/Data/DataCollectionTemplate.xlsx
+++ b/Data/DataCollectionTemplate.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="94">
   <si>
     <t>Glue</t>
   </si>
@@ -298,6 +298,9 @@
   </si>
   <si>
     <t>DeeActor</t>
+  </si>
+  <si>
+    <t>DeeBoyfriend</t>
   </si>
 </sst>
 </file>
@@ -909,10 +912,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G67"/>
+  <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F38" sqref="F4:F38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -928,7 +931,6 @@
       <c r="A1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="1"/>
     </row>
     <row r="3" spans="1:6" ht="17">
       <c r="C3" s="2" t="s">
@@ -1395,12 +1397,17 @@
         <v>92</v>
       </c>
     </row>
-    <row r="67" spans="2:7" ht="152" customHeight="1">
-      <c r="E67" s="6" t="s">
+    <row r="67" spans="2:7">
+      <c r="B67" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" ht="152" customHeight="1">
+      <c r="E68" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="F67" s="7"/>
-      <c r="G67" s="7"/>
+      <c r="F68" s="7"/>
+      <c r="G68" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>